<commit_message>
Modified column name to remove _
</commit_message>
<xml_diff>
--- a/Project 2 - V2.xlsx
+++ b/Project 2 - V2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel-i5-6600K\Documents\EvolveU\Project2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EvolveU\Project2\POS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5397CD-F7EF-4F79-A55B-95BF93F2C88C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C7E6F2-4469-4559-9EEE-336E4AA1F4AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1258,13 +1258,13 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Address_1</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Address_2</a:t>
+            <a:t>- Address1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- Address2</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1286,19 +1286,19 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Postal_Code</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Phone_Number</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Contact_Person</a:t>
+            <a:t>- PostalCode</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- PhoneNumber</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- ContactPerson</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1310,13 +1310,13 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Date_Added</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Last_Update_Date</a:t>
+            <a:t>- DateAdded</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- LastUpdateDate</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1332,7 +1332,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:colOff>476250</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -1350,7 +1350,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="15525750" y="733425"/>
-          <a:ext cx="1314450" cy="1819275"/>
+          <a:ext cx="1409700" cy="1819275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1410,13 +1410,13 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Product_Category</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Supplier_ID</a:t>
+            <a:t>- ProductCategoryID</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- SupplierID</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1428,7 +1428,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Date_Added</a:t>
+            <a:t>- DateAdded</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1438,7 +1438,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>_Update_Date</a:t>
+            <a:t>UpdateDate</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100"/>
         </a:p>
@@ -1521,13 +1521,13 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Company_Name</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Address_1</a:t>
+            <a:t>- CompanyName</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- Address1</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1537,7 +1537,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>_2</a:t>
+            <a:t>2</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1555,25 +1555,25 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>- Postal_Code</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>- Phone_Number</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>- Contact_Person</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Contact_</a:t>
+            <a:t>- PostalCode</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>- PhoneNumber</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>- ContactPerson</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- Contact</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
@@ -1590,7 +1590,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Date_Added</a:t>
+            <a:t>- DateAdded</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1600,7 +1600,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>_Update_Date</a:t>
+            <a:t>UpdateDate</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100"/>
         </a:p>
@@ -1683,13 +1683,13 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Customer_ID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Order_Date</a:t>
+            <a:t>- CustomerID</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- OrderDate</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1701,7 +1701,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Sales_Person_ID</a:t>
+            <a:t>- SalesPersonID</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1713,7 +1713,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Date_Added</a:t>
+            <a:t>- DateAdded</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1723,7 +1723,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>_Update_Date</a:t>
+            <a:t>UpdateDate</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100"/>
         </a:p>
@@ -1806,13 +1806,13 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Order_ID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Product_ID</a:t>
+            <a:t>- OrderID</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- ProductID</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1830,7 +1830,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Date_Added</a:t>
+            <a:t>- DateAdded</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1840,7 +1840,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>_Update_Date</a:t>
+            <a:t>UpdateDate</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100"/>
         </a:p>
@@ -1923,23 +1923,23 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Product_ID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Quantity_On</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>_Hand</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>- Quantity_Treshold</a:t>
+            <a:t>- ProductID</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- QuantityOn</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>Hand</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>- QuantityTreshold</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100"/>
         </a:p>
@@ -1962,7 +1962,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>_Update_Date</a:t>
+            <a:t>UpdateDate</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100"/>
         </a:p>
@@ -2045,26 +2045,26 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Device_ID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Company_Name</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Address_1</a:t>
+            <a:t>- DeviceID</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- CompanyName</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- Address1</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>- Address_2</a:t>
+            <a:t>- Address2</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2082,13 +2082,13 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Postal_Code</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Phone_Number</a:t>
+            <a:t>- PostalCode</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- PhoneNumber</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2100,7 +2100,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Date_Added</a:t>
+            <a:t>- DateAdded</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2110,7 +2110,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>_Update_Date</a:t>
+            <a:t>UpdateDate</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100"/>
         </a:p>
@@ -2211,7 +2211,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Date_Added</a:t>
+            <a:t>- DateAdded</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2221,7 +2221,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>_Update_Date</a:t>
+            <a:t>UpdateDate</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100"/>
         </a:p>
@@ -2304,11 +2304,11 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Transction_</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>Type_</a:t>
+            <a:t>- Transction</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>Type</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
@@ -2322,27 +2322,27 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>_ID</a:t>
+            <a:t>ID</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Quantity_On_Hand</a:t>
+            <a:t>- QuantityOnHand</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>- Quantity_Added</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>- Quantity_Taken</a:t>
+            <a:t>- QuantityAdded</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>- QuantityTaken</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100"/>
         </a:p>
@@ -2355,13 +2355,13 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- User_Id</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Date_Added</a:t>
+            <a:t>- UserId</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- DateAdded</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2371,7 +2371,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>_Update_Date</a:t>
+            <a:t>UpdateDate</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100"/>
         </a:p>
@@ -2460,7 +2460,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- First_Name</a:t>
+            <a:t>- FirstName</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2470,13 +2470,13 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>_Name</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>- Level_ID</a:t>
+            <a:t>Name</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>- LevelID</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2495,7 +2495,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Date_Added</a:t>
+            <a:t>- DateAdded</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2505,7 +2505,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>_Update_Date</a:t>
+            <a:t>UpdateDate</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100"/>
         </a:p>
@@ -2609,7 +2609,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t> Authority_Level</a:t>
+            <a:t> AuthorityLevel</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100"/>
         </a:p>
@@ -2622,7 +2622,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Date_Added</a:t>
+            <a:t>- DateAdded</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2632,7 +2632,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>_Update_Date</a:t>
+            <a:t>UpdateDate</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100"/>
         </a:p>
@@ -2733,7 +2733,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Date_Added</a:t>
+            <a:t>- DateAdded</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2743,7 +2743,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>_Update_Date</a:t>
+            <a:t>UpdateDate</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100"/>
         </a:p>
@@ -3879,8 +3879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
+      <selection activeCell="AG26" sqref="AG26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>